<commit_message>
Code ver 3.0: Change Blynk configurations, add fuzzy control for pump and normal control for light
</commit_message>
<xml_diff>
--- a/measurement_1week.xlsx
+++ b/measurement_1week.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>SOILMS</t>
   </si>
@@ -83,46 +83,76 @@
     <t>7/Evening</t>
   </si>
   <si>
-    <t>667-&gt;286</t>
-  </si>
-  <si>
-    <t>116-&gt;84</t>
-  </si>
-  <si>
-    <t>368-&gt;117</t>
-  </si>
-  <si>
-    <t>241-&gt;197</t>
-  </si>
-  <si>
-    <t>288-&gt;211</t>
-  </si>
-  <si>
-    <t>303-&gt;201</t>
-  </si>
-  <si>
-    <t>346-&gt;201</t>
-  </si>
-  <si>
-    <t>366-&gt;246</t>
-  </si>
-  <si>
-    <t>340-&gt;265</t>
-  </si>
-  <si>
-    <t>369-&gt;291</t>
-  </si>
-  <si>
-    <t>387-&gt;292</t>
-  </si>
-  <si>
-    <t>389-&gt;298</t>
-  </si>
-  <si>
-    <t>420-&gt;302</t>
-  </si>
-  <si>
-    <t>433-&gt;379</t>
+    <t>Fuzzy calculations</t>
+  </si>
+  <si>
+    <t>Rule 1 A</t>
+  </si>
+  <si>
+    <t>Rule 1 B</t>
+  </si>
+  <si>
+    <t>Rule 2 A</t>
+  </si>
+  <si>
+    <t>Rule 2 B</t>
+  </si>
+  <si>
+    <t>Rule 3 A</t>
+  </si>
+  <si>
+    <t>Rule 3 B</t>
+  </si>
+  <si>
+    <t>Rule 4 A</t>
+  </si>
+  <si>
+    <t>Rule 4 B</t>
+  </si>
+  <si>
+    <t>Rule 5 A</t>
+  </si>
+  <si>
+    <t>Rule 6 A</t>
+  </si>
+  <si>
+    <t>Rule 6 B</t>
+  </si>
+  <si>
+    <t>SOILAF</t>
+  </si>
+  <si>
+    <t>Rule 1 S</t>
+  </si>
+  <si>
+    <t>Rule 2 S</t>
+  </si>
+  <si>
+    <t>Rule 3 S</t>
+  </si>
+  <si>
+    <t>Rule 4 S</t>
+  </si>
+  <si>
+    <t>Rule 5 S</t>
+  </si>
+  <si>
+    <t>Rule 6 S</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>PUM MED</t>
+  </si>
+  <si>
+    <t>PUM HI</t>
+  </si>
+  <si>
+    <t>PUM OFF</t>
+  </si>
+  <si>
+    <t>PUM LOW</t>
   </si>
 </sst>
 </file>
@@ -139,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,6 +185,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -186,11 +222,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
@@ -505,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEF182A-D678-4CE2-8070-BCF253692FFB}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -658,94 +698,1432 @@
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>32</v>
+      <c r="B4" s="2">
+        <v>667</v>
+      </c>
+      <c r="C4" s="1">
+        <v>116</v>
+      </c>
+      <c r="D4" s="1">
+        <v>368</v>
+      </c>
+      <c r="E4" s="1">
+        <v>241</v>
+      </c>
+      <c r="F4" s="1">
+        <v>288</v>
+      </c>
+      <c r="G4" s="1">
+        <v>303</v>
+      </c>
+      <c r="H4" s="1">
+        <v>346</v>
+      </c>
+      <c r="I4" s="1">
+        <v>366</v>
+      </c>
+      <c r="J4" s="1">
+        <v>340</v>
+      </c>
+      <c r="K4" s="1">
+        <v>369</v>
+      </c>
+      <c r="L4" s="1">
+        <v>387</v>
+      </c>
+      <c r="M4" s="1">
+        <v>389</v>
+      </c>
+      <c r="N4" s="2">
+        <v>420</v>
+      </c>
+      <c r="O4" s="2">
+        <v>433</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1">
+        <v>286</v>
+      </c>
+      <c r="C5" s="1">
+        <v>84</v>
+      </c>
+      <c r="D5" s="1">
+        <v>117</v>
+      </c>
+      <c r="E5" s="1">
+        <v>197</v>
+      </c>
+      <c r="F5" s="1">
+        <v>211</v>
+      </c>
+      <c r="G5" s="1">
+        <v>201</v>
+      </c>
+      <c r="H5" s="1">
+        <v>201</v>
+      </c>
+      <c r="I5" s="1">
+        <v>246</v>
+      </c>
+      <c r="J5" s="1">
+        <v>265</v>
+      </c>
+      <c r="K5" s="1">
+        <v>291</v>
+      </c>
+      <c r="L5" s="1">
+        <v>292</v>
+      </c>
+      <c r="M5" s="1">
+        <v>298</v>
+      </c>
+      <c r="N5" s="1">
+        <v>302</v>
+      </c>
+      <c r="O5" s="1">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>277</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>129</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D6" s="1">
         <v>340</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E6" s="1">
         <v>27</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F6" s="1">
         <v>377</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G6" s="1">
         <v>14</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H6" s="1">
         <v>292</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I6" s="1">
         <v>15</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J6" s="1">
         <v>397</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K6" s="1">
         <v>9</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L6" s="1">
         <v>204</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M6" s="1">
         <v>3</v>
       </c>
-      <c r="N5" s="1">
+      <c r="N6" s="1">
         <v>448</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O6" s="1">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <f>MAX(0,MIN(1,(0.01*B4)-4))</f>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:O10" si="0">MAX(0,MIN(1,(0.01*C4)-4))</f>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>0.33000000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <f>(-0.05*B2)+3.5</f>
+        <v>0.59999999999999964</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:O11" si="1">(-0.05*C2)+3.5</f>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>0.59999999999999964</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0.84999999999999964</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>0.69999999999999973</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>0.44999999999999973</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>0.44999999999999973</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>0.59999999999999964</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>0.54999999999999982</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="6">
+        <f>MIN(B10,B11)</f>
+        <v>0.59999999999999964</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" ref="C12:O12" si="2">MIN(C10,C11)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="6">
+        <f t="shared" si="2"/>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="O12" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <f>MAX(0,MIN(1,(-0.01*B4)+4))</f>
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:O13" si="3">MAX(0,MIN(1,(-0.01*C4)+4))</f>
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="3"/>
+        <v>0.31999999999999984</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>0.96999999999999975</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>0.54</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>0.33999999999999986</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="3"/>
+        <v>0.31000000000000005</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>0.12999999999999989</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>0.10999999999999988</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <f>(-0.05*B2)+3.5</f>
+        <v>0.59999999999999964</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:O14" si="4">(-0.05*C2)+3.5</f>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="4"/>
+        <v>0.59999999999999964</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="4"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>0.84999999999999964</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="4"/>
+        <v>0.69999999999999973</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>0.44999999999999973</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>0.44999999999999973</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="4"/>
+        <v>0.59999999999999964</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="4"/>
+        <v>0.54999999999999982</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="6">
+        <f>MIN(B13,B14)</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" ref="C15:O15" si="5">MIN(C13,C14)</f>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="D15" s="6">
+        <f t="shared" si="5"/>
+        <v>0.31999999999999984</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="5"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="5"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" si="5"/>
+        <v>0.84999999999999964</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" si="5"/>
+        <v>0.54</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" si="5"/>
+        <v>0.33999999999999986</v>
+      </c>
+      <c r="J15" s="6">
+        <f t="shared" si="5"/>
+        <v>0.44999999999999973</v>
+      </c>
+      <c r="K15" s="6">
+        <f t="shared" si="5"/>
+        <v>0.31000000000000005</v>
+      </c>
+      <c r="L15" s="6">
+        <f t="shared" si="5"/>
+        <v>0.12999999999999989</v>
+      </c>
+      <c r="M15" s="6">
+        <f t="shared" si="5"/>
+        <v>0.10999999999999988</v>
+      </c>
+      <c r="N15" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <f>MAX(0,MIN(1,(-0.01*B4)+4))</f>
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:O16" si="6">MAX(0,MIN(1,(-0.01*C4)+4))</f>
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="6"/>
+        <v>0.31999999999999984</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="6"/>
+        <v>0.96999999999999975</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="6"/>
+        <v>0.54</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="6"/>
+        <v>0.33999999999999986</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="6"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="6"/>
+        <v>0.31000000000000005</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="6"/>
+        <v>0.12999999999999989</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="6"/>
+        <v>0.10999999999999988</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <f>(0.05*B2)-2.5</f>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:O17" si="7">(0.05*C2)-2.5</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="7"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="7"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="7"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="7"/>
+        <v>0.15000000000000036</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="7"/>
+        <v>0.30000000000000027</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="7"/>
+        <v>0.25</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="7"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="7"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="7"/>
+        <v>0.75</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="7"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="7"/>
+        <v>0.45000000000000018</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="6">
+        <f>MIN(B16,B17)</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" ref="C18:O18" si="8">MIN(C16,C17)</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="D18" s="6">
+        <f t="shared" si="8"/>
+        <v>0.31999999999999984</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="8"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="8"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" si="8"/>
+        <v>0.15000000000000036</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="8"/>
+        <v>0.30000000000000027</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="8"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" si="8"/>
+        <v>0.31000000000000005</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="8"/>
+        <v>0.12999999999999989</v>
+      </c>
+      <c r="M18" s="6">
+        <f t="shared" si="8"/>
+        <v>0.10999999999999988</v>
+      </c>
+      <c r="N18" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <f>MAX(0,MIN(1,(-0.01*B4)+5))</f>
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <f>MAX(0,MIN(1,(0.01*C4)-3))</f>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:M19" si="9">MAX(0,MIN(1,(0.01*D4)-3))</f>
+        <v>0.68000000000000016</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="9"/>
+        <v>3.0000000000000249E-2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="9"/>
+        <v>0.45999999999999996</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="9"/>
+        <v>0.66000000000000014</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="9"/>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="9"/>
+        <v>0.69</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="9"/>
+        <v>0.87000000000000011</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="9"/>
+        <v>0.89000000000000012</v>
+      </c>
+      <c r="N19">
+        <f>MAX(0,MIN(1,(-0.01*N4)+5))</f>
+        <v>0.79999999999999982</v>
+      </c>
+      <c r="O19">
+        <f>MAX(0,MIN(1,(-0.01*O4)+5))</f>
+        <v>0.66999999999999993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20">
+        <f>(0.05*B2)-2.5</f>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:O20" si="10">(0.05*C2)-2.5</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="10"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="10"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="10"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="10"/>
+        <v>0.15000000000000036</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="10"/>
+        <v>0.30000000000000027</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="10"/>
+        <v>0.25</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="10"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="10"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="10"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="10"/>
+        <v>0.45000000000000018</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="6">
+        <f>MIN(B19,B20)</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="6">
+        <f t="shared" ref="C21:O21" si="11">MIN(C19,C20)</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="6">
+        <f t="shared" si="11"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
+        <f t="shared" si="11"/>
+        <v>3.0000000000000249E-2</v>
+      </c>
+      <c r="H21" s="6">
+        <f t="shared" si="11"/>
+        <v>0.30000000000000027</v>
+      </c>
+      <c r="I21" s="6">
+        <f t="shared" si="11"/>
+        <v>0.25</v>
+      </c>
+      <c r="J21" s="6">
+        <f t="shared" si="11"/>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="K21" s="6">
+        <f t="shared" si="11"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="L21" s="6">
+        <f t="shared" si="11"/>
+        <v>0.75</v>
+      </c>
+      <c r="M21" s="6">
+        <f t="shared" si="11"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="N21" s="6">
+        <f t="shared" si="11"/>
+        <v>0.45000000000000018</v>
+      </c>
+      <c r="O21" s="6">
+        <f t="shared" si="11"/>
+        <v>0.66999999999999993</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="4">
+        <f>(0.0666667*B3)-1.66667</f>
+        <v>0.3333309999999996</v>
+      </c>
+      <c r="C22" s="4">
+        <f t="shared" ref="C22:O22" si="12">(0.0666667*C3)-1.66667</f>
+        <v>0.26666429999999974</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="12"/>
+        <v>0.19999759999999989</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="12"/>
+        <v>0.19999759999999989</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="12"/>
+        <v>0.13333089999999981</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" si="12"/>
+        <v>0.3333309999999996</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="12"/>
+        <v>0.13333089999999981</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="12"/>
+        <v>0.26666429999999974</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="12"/>
+        <v>0.13333089999999981</v>
+      </c>
+      <c r="K22" s="4">
+        <f t="shared" si="12"/>
+        <v>0.19999759999999989</v>
+      </c>
+      <c r="L22" s="4">
+        <f t="shared" si="12"/>
+        <v>0.13333089999999981</v>
+      </c>
+      <c r="M22" s="4">
+        <f t="shared" si="12"/>
+        <v>0.3333309999999996</v>
+      </c>
+      <c r="N22" s="4">
+        <f t="shared" si="12"/>
+        <v>0.19999759999999989</v>
+      </c>
+      <c r="O22" s="4">
+        <f t="shared" si="12"/>
+        <v>0.19999759999999989</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="7">
+        <f>B22</f>
+        <v>0.3333309999999996</v>
+      </c>
+      <c r="C23" s="7">
+        <f t="shared" ref="C23:O23" si="13">C22</f>
+        <v>0.26666429999999974</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="13"/>
+        <v>0.19999759999999989</v>
+      </c>
+      <c r="E23" s="7">
+        <f t="shared" si="13"/>
+        <v>0.19999759999999989</v>
+      </c>
+      <c r="F23" s="7">
+        <f t="shared" si="13"/>
+        <v>0.13333089999999981</v>
+      </c>
+      <c r="G23" s="7">
+        <f t="shared" si="13"/>
+        <v>0.3333309999999996</v>
+      </c>
+      <c r="H23" s="7">
+        <f t="shared" si="13"/>
+        <v>0.13333089999999981</v>
+      </c>
+      <c r="I23" s="7">
+        <f t="shared" si="13"/>
+        <v>0.26666429999999974</v>
+      </c>
+      <c r="J23" s="7">
+        <f t="shared" si="13"/>
+        <v>0.13333089999999981</v>
+      </c>
+      <c r="K23" s="7">
+        <f t="shared" si="13"/>
+        <v>0.19999759999999989</v>
+      </c>
+      <c r="L23" s="7">
+        <f t="shared" si="13"/>
+        <v>0.13333089999999981</v>
+      </c>
+      <c r="M23" s="7">
+        <f t="shared" si="13"/>
+        <v>0.3333309999999996</v>
+      </c>
+      <c r="N23" s="7">
+        <f t="shared" si="13"/>
+        <v>0.19999759999999989</v>
+      </c>
+      <c r="O23" s="7">
+        <f t="shared" si="13"/>
+        <v>0.19999759999999989</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="4">
+        <f>(-0.0666667*B3)+2.66667</f>
+        <v>0.66666900000000018</v>
+      </c>
+      <c r="C24" s="4">
+        <f t="shared" ref="C24:O24" si="14">(-0.0666667*C3)+2.66667</f>
+        <v>0.73333570000000003</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" si="14"/>
+        <v>0.80000239999999989</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="14"/>
+        <v>0.80000239999999989</v>
+      </c>
+      <c r="F24" s="4">
+        <f t="shared" si="14"/>
+        <v>0.86666909999999997</v>
+      </c>
+      <c r="G24" s="4">
+        <f t="shared" si="14"/>
+        <v>0.66666900000000018</v>
+      </c>
+      <c r="H24" s="4">
+        <f t="shared" si="14"/>
+        <v>0.86666909999999997</v>
+      </c>
+      <c r="I24" s="4">
+        <f t="shared" si="14"/>
+        <v>0.73333570000000003</v>
+      </c>
+      <c r="J24" s="4">
+        <f t="shared" si="14"/>
+        <v>0.86666909999999997</v>
+      </c>
+      <c r="K24" s="4">
+        <f t="shared" si="14"/>
+        <v>0.80000239999999989</v>
+      </c>
+      <c r="L24" s="4">
+        <f t="shared" si="14"/>
+        <v>0.86666909999999997</v>
+      </c>
+      <c r="M24" s="4">
+        <f t="shared" si="14"/>
+        <v>0.66666900000000018</v>
+      </c>
+      <c r="N24" s="4">
+        <f t="shared" si="14"/>
+        <v>0.80000239999999989</v>
+      </c>
+      <c r="O24" s="4">
+        <f t="shared" si="14"/>
+        <v>0.80000239999999989</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <f>(0.05*B2)-2.5</f>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:O25" si="15">(0.05*C2)-2.5</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="15"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="15"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="15"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="15"/>
+        <v>0.15000000000000036</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="15"/>
+        <v>0.30000000000000027</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="15"/>
+        <v>0.25</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="15"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="15"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="15"/>
+        <v>0.75</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="15"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="15"/>
+        <v>0.45000000000000018</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="7">
+        <f>MIN(B24,B25)</f>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="C26" s="7">
+        <f t="shared" ref="C26:O26" si="16">MIN(C24,C25)</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="16"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="E26" s="7">
+        <f t="shared" si="16"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="F26" s="7">
+        <f t="shared" si="16"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="G26" s="7">
+        <f t="shared" si="16"/>
+        <v>0.15000000000000036</v>
+      </c>
+      <c r="H26" s="7">
+        <f t="shared" si="16"/>
+        <v>0.30000000000000027</v>
+      </c>
+      <c r="I26" s="7">
+        <f t="shared" si="16"/>
+        <v>0.25</v>
+      </c>
+      <c r="J26" s="7">
+        <f t="shared" si="16"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="K26" s="7">
+        <f t="shared" si="16"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="L26" s="7">
+        <f t="shared" si="16"/>
+        <v>0.75</v>
+      </c>
+      <c r="M26" s="7">
+        <f t="shared" si="16"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="N26" s="7">
+        <f t="shared" si="16"/>
+        <v>0.45000000000000018</v>
+      </c>
+      <c r="O26" s="7">
+        <f t="shared" si="16"/>
+        <v>0.80000239999999989</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="4">
+        <f>MAX(B23,B26)</f>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="C28" s="4">
+        <f t="shared" ref="C28:O28" si="17">MAX(C23,C26)</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="17"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" si="17"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="17"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="G28" s="4">
+        <f t="shared" si="17"/>
+        <v>0.3333309999999996</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="17"/>
+        <v>0.30000000000000027</v>
+      </c>
+      <c r="I28" s="4">
+        <f t="shared" si="17"/>
+        <v>0.26666429999999974</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" si="17"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="K28" s="4">
+        <f t="shared" si="17"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="L28" s="4">
+        <f t="shared" si="17"/>
+        <v>0.75</v>
+      </c>
+      <c r="M28" s="4">
+        <f t="shared" si="17"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="N28" s="4">
+        <f t="shared" si="17"/>
+        <v>0.45000000000000018</v>
+      </c>
+      <c r="O28" s="4">
+        <f t="shared" si="17"/>
+        <v>0.80000239999999989</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29">
+        <f>MAX(B18,B21)</f>
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:O29" si="18">MAX(C18,C21)</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="18"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="18"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="18"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="18"/>
+        <v>0.15000000000000036</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="18"/>
+        <v>0.30000000000000027</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="18"/>
+        <v>0.25</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="18"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="18"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="18"/>
+        <v>0.75</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="18"/>
+        <v>0.40000000000000036</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="18"/>
+        <v>0.45000000000000018</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="18"/>
+        <v>0.66999999999999993</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <f>B15</f>
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:O30" si="19">C15</f>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="19"/>
+        <v>0.31999999999999984</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="19"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="19"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="19"/>
+        <v>0.84999999999999964</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="19"/>
+        <v>0.54</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="19"/>
+        <v>0.33999999999999986</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="19"/>
+        <v>0.44999999999999973</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="19"/>
+        <v>0.31000000000000005</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="19"/>
+        <v>0.12999999999999989</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="19"/>
+        <v>0.10999999999999988</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <f>B12</f>
+        <v>0.59999999999999964</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ref="C31:O31" si="20">C12</f>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="20"/>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="20"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>